<commit_message>
actualizacion enero 10-2025 despues de la reunion
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="cuota-extra" sheetId="1" state="visible" r:id="rId3"/>
@@ -279,7 +279,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -408,8 +408,8 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -499,7 +499,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>0</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,7 +554,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>0</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,7 +642,7 @@
         <v>42</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>0</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2761,51 +2761,51 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0" t="n">
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="C3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualizacion recaudo de enero 14 de 2025
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cuota-extra" sheetId="1" state="visible" r:id="rId3"/>
@@ -406,9 +406,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -665,6 +665,11 @@
       </c>
       <c r="C23" s="1" t="n">
         <v>20000</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D31" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -685,8 +690,8 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -755,7 +760,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0</v>
@@ -783,7 +788,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0</v>
@@ -867,7 +872,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>0</v>
+        <v>56000</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>0</v>
@@ -937,7 +942,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>0</v>
@@ -979,7 +984,7 @@
         <v>42</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
actualizacion enero 15 2025 - 8:50
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cuota-extra" sheetId="1" state="visible" r:id="rId3"/>
@@ -412,8 +412,8 @@
   </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -692,8 +692,8 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -748,7 +748,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0</v>
@@ -818,7 +818,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0</v>
@@ -832,10 +832,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,7 +902,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0</v>
@@ -916,7 +916,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>
@@ -930,7 +930,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>0</v>
@@ -958,7 +958,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>0</v>
@@ -972,7 +972,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>0</v>
@@ -1014,7 +1014,7 @@
         <v>46</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
actualizacion enero 17 de 025
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -693,7 +693,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -720,7 +720,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -888,7 +888,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>0</v>
@@ -2821,8 +2821,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualizacion cuota extra claudia
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="cuota-extra" sheetId="1" state="visible" r:id="rId3"/>
@@ -412,8 +412,8 @@
   </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -624,7 +624,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>0</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,7 +692,7 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
actualizacion enero 18 de 2025
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cuota-extra" sheetId="1" state="visible" r:id="rId3"/>
@@ -412,7 +412,7 @@
   </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -692,8 +692,8 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -734,7 +734,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0</v>
@@ -804,7 +804,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>0</v>
@@ -846,7 +846,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>0</v>
@@ -1038,7 +1038,7 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1384,7 +1384,7 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -1730,7 +1730,7 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2076,7 +2076,7 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -2422,7 +2422,7 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2768,7 +2768,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ajustes fin de mes enero
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="56">
   <si>
     <t xml:space="preserve">placa</t>
   </si>
@@ -690,10 +690,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -723,7 +723,7 @@
         <v>65000</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,7 +737,7 @@
         <v>65000</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,7 +751,7 @@
         <v>65000</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -765,7 +765,7 @@
         <v>65000</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -776,10 +776,10 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,7 +793,7 @@
         <v>65000</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -807,7 +807,7 @@
         <v>65000</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,7 +821,7 @@
         <v>65000</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -849,43 +849,43 @@
         <v>65000</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>0</v>
+        <v>56000</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0</v>
+        <v>56000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>56000</v>
+        <v>65000</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>56000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>65000</v>
@@ -896,94 +896,94 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>65000</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>65000</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>65000</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>65000</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>65000</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>65000</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>65000</v>
@@ -994,30 +994,16 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>65000</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
   </sheetData>
@@ -1036,10 +1022,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1200,10 +1186,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -1214,10 +1200,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -1228,10 +1214,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -1242,10 +1228,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -1256,10 +1242,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -1270,10 +1256,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
@@ -1284,10 +1270,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0</v>
@@ -1298,10 +1284,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0</v>
@@ -1312,10 +1298,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0</v>
@@ -1326,10 +1312,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
@@ -1340,29 +1326,15 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1382,10 +1354,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1546,10 +1518,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -1560,10 +1532,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -1574,10 +1546,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -1588,10 +1560,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -1602,10 +1574,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -1616,10 +1588,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
@@ -1630,10 +1602,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0</v>
@@ -1644,10 +1616,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0</v>
@@ -1658,10 +1630,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0</v>
@@ -1672,10 +1644,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
@@ -1686,29 +1658,15 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1728,10 +1686,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1892,10 +1850,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -1906,10 +1864,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -1920,10 +1878,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -1934,10 +1892,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -1948,10 +1906,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -1962,10 +1920,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
@@ -1976,10 +1934,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0</v>
@@ -1990,10 +1948,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0</v>
@@ -2004,10 +1962,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0</v>
@@ -2018,10 +1976,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
@@ -2032,29 +1990,15 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2074,10 +2018,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2238,10 +2182,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -2252,10 +2196,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -2266,10 +2210,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -2280,10 +2224,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -2294,10 +2238,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -2308,10 +2252,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
@@ -2322,10 +2266,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0</v>
@@ -2336,10 +2280,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0</v>
@@ -2350,10 +2294,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0</v>
@@ -2364,10 +2308,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
@@ -2378,29 +2322,15 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2420,10 +2350,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2584,10 +2514,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -2598,10 +2528,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -2612,10 +2542,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -2626,10 +2556,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -2640,10 +2570,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -2654,10 +2584,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
@@ -2668,10 +2598,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0</v>
@@ -2682,10 +2612,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0</v>
@@ -2696,10 +2626,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0</v>
@@ -2710,10 +2640,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
@@ -2724,29 +2654,15 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2821,8 +2737,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actualizacion feb 17 - 23:06
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="59">
   <si>
     <t xml:space="preserve">placa</t>
   </si>
@@ -180,29 +180,7 @@
     <t xml:space="preserve">33-73</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Rafael </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(casa desocupada)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Rafael</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rafael </t>
+    <t xml:space="preserve">Rafael (casa desocupada)</t>
   </si>
   <si>
     <t xml:space="preserve">Vigilante</t>
@@ -237,7 +215,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -258,11 +236,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -344,15 +317,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1094,7 +1067,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1121,7 +1094,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -1135,7 +1108,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0</v>
@@ -1149,7 +1122,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0</v>
@@ -1163,7 +1136,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0</v>
@@ -1191,7 +1164,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0</v>
@@ -1219,7 +1192,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0</v>
@@ -1233,10 +1206,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1275,10 +1248,10 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1303,7 +1276,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0</v>
@@ -1317,7 +1290,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>
@@ -1331,7 +1304,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>0</v>
@@ -1345,7 +1318,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>0</v>
@@ -1373,7 +1346,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>0</v>
@@ -1387,10 +1360,10 @@
         <v>50</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,10 +1374,10 @@
         <v>42</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1415,7 +1388,7 @@
         <v>44</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>0</v>
@@ -1429,7 +1402,7 @@
         <v>46</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>0</v>
@@ -1451,7 +1424,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1615,10 +1588,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -1629,10 +1602,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -1643,10 +1616,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -1657,10 +1630,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -1671,10 +1644,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -1685,10 +1658,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
@@ -1699,10 +1672,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0</v>
@@ -1713,10 +1686,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0</v>
@@ -1727,10 +1700,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0</v>
@@ -1741,10 +1714,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
@@ -1755,10 +1728,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0</v>
@@ -1769,15 +1742,29 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="n">
+      <c r="C24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1797,7 +1784,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -1961,10 +1948,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -1975,10 +1962,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -1989,10 +1976,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -2003,10 +1990,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -2017,10 +2004,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -2031,10 +2018,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
@@ -2045,10 +2032,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0</v>
@@ -2059,10 +2046,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0</v>
@@ -2073,10 +2060,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0</v>
@@ -2087,10 +2074,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
@@ -2101,10 +2088,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0</v>
@@ -2115,15 +2102,29 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="n">
+      <c r="C24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2143,7 +2144,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -2307,10 +2308,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -2321,10 +2322,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -2335,10 +2336,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -2349,10 +2350,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -2363,10 +2364,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -2377,10 +2378,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
@@ -2391,10 +2392,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0</v>
@@ -2405,10 +2406,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0</v>
@@ -2419,10 +2420,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0</v>
@@ -2433,10 +2434,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
@@ -2447,10 +2448,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0</v>
@@ -2461,15 +2462,29 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="n">
+      <c r="C24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2489,10 +2504,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2653,10 +2668,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -2667,10 +2682,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -2681,10 +2696,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -2695,10 +2710,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -2709,10 +2724,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -2723,10 +2738,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
@@ -2737,10 +2752,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>0</v>
@@ -2751,10 +2766,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>0</v>
@@ -2765,10 +2780,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>0</v>
@@ -2779,10 +2794,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>0</v>
@@ -2793,10 +2808,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0</v>
@@ -2807,15 +2822,29 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1" t="n">
+      <c r="C24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2845,24 +2874,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0</v>
@@ -2873,10 +2902,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>0</v>
@@ -2915,7 +2944,7 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
actualizacion feb 18 20.58
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1150,7 +1150,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0</v>
@@ -1178,7 +1178,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>0</v>
@@ -1234,7 +1234,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>0</v>
@@ -1262,10 +1262,10 @@
         <v>28</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1332,7 +1332,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
actualizacion a marzo 2 de 2025
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1111,7 +1111,7 @@
         <v>65000</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,7 +1125,7 @@
         <v>65000</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1139,7 +1139,7 @@
         <v>65000</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1153,7 +1153,7 @@
         <v>65000</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1223,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1293,7 +1293,7 @@
         <v>65000</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1307,7 +1307,7 @@
         <v>65000</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,7 +1391,7 @@
         <v>65000</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1405,7 +1405,7 @@
         <v>65000</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
   </sheetData>
@@ -1427,7 +1427,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1650,7 +1650,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
actualizacion marzo 5 de 2025
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1097,7 +1097,7 @@
         <v>65000</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,7 +1167,7 @@
         <v>65000</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1181,7 +1181,7 @@
         <v>65000</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1195,7 +1195,7 @@
         <v>65000</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,7 +1237,7 @@
         <v>65000</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1279,7 +1279,7 @@
         <v>65000</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1335,7 +1335,7 @@
         <v>65000</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1349,7 +1349,7 @@
         <v>65000</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
ajustes 1ra quincena mar
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1427,7 +1427,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1454,7 +1454,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0</v>
+        <v>32500</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>0</v>
@@ -1468,7 +1468,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0</v>
@@ -1482,7 +1482,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0</v>
@@ -1496,7 +1496,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0</v>
@@ -1524,7 +1524,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>0</v>
@@ -1552,7 +1552,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>0</v>
@@ -1566,10 +1566,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,10 +1622,10 @@
         <v>28</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1636,7 +1636,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0</v>
@@ -1664,7 +1664,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>0</v>
@@ -1706,7 +1706,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>0</v>
@@ -1720,10 +1720,10 @@
         <v>50</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>0</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,7 +1762,7 @@
         <v>46</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
ajustes mar 19 - 21:14
</commit_message>
<xml_diff>
--- a/docs/vecinos.xlsx
+++ b/docs/vecinos.xlsx
@@ -1427,7 +1427,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1510,7 +1510,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0</v>

</xml_diff>